<commit_message>
Adding maven surefire plugin
</commit_message>
<xml_diff>
--- a/resources/SampleTestFile.xlsx
+++ b/resources/SampleTestFile.xlsx
@@ -4,6 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Sheet2" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,43 +12,79 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+  <si>
+    <t>User Name</t>
+  </si>
+  <si>
+    <t>User Repo</t>
+  </si>
+  <si>
+    <t>User Repo URL</t>
+  </si>
   <si>
     <t>shivam</t>
   </si>
   <si>
-    <t>WebApp</t>
-  </si>
-  <si>
-    <t>https://github.com/shivamgupta2607/WebApp</t>
-  </si>
-  <si>
-    <t>DemoSampleWebApp</t>
-  </si>
-  <si>
-    <t>https://github.com/skshukla/DemoSampleWebApp.git</t>
+    <t>MyTest</t>
+  </si>
+  <si>
+    <t>https://github.com/shivamgupta2607/MyTest</t>
   </si>
   <si>
     <t>sachin</t>
+  </si>
+  <si>
+    <t>Test Case Repo</t>
+  </si>
+  <si>
+    <t>Test Case Repo URL</t>
+  </si>
+  <si>
+    <t>interviews</t>
+  </si>
+  <si>
+    <t>git@repo2.deskera.com:infinity-stones/interviews.git</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="9">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
-    <font>
+    <font>
+      <b/>
+    </font>
+    <font>
+      <b/>
       <u/>
       <color rgb="FF1155CC"/>
     </font>
     <font>
+      <b/>
       <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF1155CC"/>
+    </font>
+    <font/>
+    <font>
+      <b/>
+      <color rgb="FF000000"/>
+    </font>
+    <font>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -65,7 +102,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -75,7 +112,20 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -87,6 +137,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -295,7 +349,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="2" max="2" width="38.43"/>
-    <col customWidth="1" min="3" max="3" width="39.57"/>
+    <col customWidth="1" min="3" max="3" width="54.0"/>
     <col customWidth="1" min="4" max="4" width="38.43"/>
     <col customWidth="1" min="5" max="5" width="59.14"/>
   </cols>
@@ -310,37 +364,115 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="2" t="s">
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>4</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="C1"/>
-    <hyperlink r:id="rId2" ref="E1"/>
-    <hyperlink r:id="rId3" ref="C2"/>
-    <hyperlink r:id="rId4" ref="E2"/>
+    <hyperlink r:id="rId1" ref="C2"/>
+    <hyperlink r:id="rId2" ref="C3"/>
   </hyperlinks>
-  <drawing r:id="rId5"/>
+  <drawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="15.29"/>
+    <col customWidth="1" min="2" max="2" width="45.14"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>